<commit_message>
added for User Module
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/team2Data.xlsx
+++ b/src/test/resources/testData/team2Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msira\Team2_AssuredNinjas\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1755C2B-CF38-4F76-9A2F-0F86A68259EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E958AF-6790-4DC0-9836-6B524AE13F48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16944" windowHeight="7608" activeTab="2" xr2:uid="{CF3C7186-C499-4D8C-A75E-155913C3CEE5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22464" windowHeight="7608" activeTab="2" xr2:uid="{CF3C7186-C499-4D8C-A75E-155913C3CEE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>scenario</t>
   </si>
@@ -191,9 +191,6 @@
     <t>endpoint</t>
   </si>
   <si>
-    <t>U37</t>
-  </si>
-  <si>
     <t>endpointusers</t>
   </si>
   <si>
@@ -258,6 +255,18 @@
   </si>
   <si>
     <t>english</t>
+  </si>
+  <si>
+    <t>U52</t>
+  </si>
+  <si>
+    <t>U60</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>U141</t>
   </si>
 </sst>
 </file>
@@ -754,10 +763,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7F299E-5826-4A76-88BE-382111C9768A}">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,13 +841,13 @@
         <v>23</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
@@ -958,7 +967,7 @@
         <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
@@ -976,73 +985,79 @@
         <v>6546</v>
       </c>
       <c r="V4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
         <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
         <v>61</v>
       </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>62</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>63</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>64</v>
-      </c>
-      <c r="F6" t="s">
-        <v>65</v>
       </c>
       <c r="G6" t="s">
         <v>40</v>
       </c>
       <c r="H6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" t="s">
         <v>67</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>68</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>69</v>
-      </c>
-      <c r="L6" t="s">
-        <v>70</v>
       </c>
       <c r="M6" t="s">
         <v>34</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="P6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="s">
         <v>72</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>73</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>74</v>
-      </c>
-      <c r="F7" t="s">
-        <v>75</v>
       </c>
       <c r="G7" t="s">
         <v>40</v>
@@ -1051,7 +1066,15 @@
         <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>